<commit_message>
took away unnecessary extra mapper bean
</commit_message>
<xml_diff>
--- a/src/main/resources/files/results/CHAMPIONS.xlsx
+++ b/src/main/resources/files/results/CHAMPIONS.xlsx
@@ -196,7 +196,7 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -223,7 +223,7 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H3" t="n">
         <v>0.0</v>
@@ -250,7 +250,7 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H4" t="n">
         <v>0.0</v>
@@ -277,7 +277,7 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H5" t="n">
         <v>0.0</v>
@@ -304,7 +304,7 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H6" t="n">
         <v>0.0</v>
@@ -331,7 +331,7 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H7" t="n">
         <v>0.0</v>
@@ -358,7 +358,7 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H8" t="n">
         <v>0.0</v>
@@ -385,7 +385,7 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H9" t="n">
         <v>0.0</v>
@@ -412,7 +412,7 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H10" t="n">
         <v>0.0</v>
@@ -439,7 +439,7 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H11" t="n">
         <v>0.0</v>
@@ -466,7 +466,7 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H12" t="n">
         <v>0.0</v>
@@ -493,7 +493,7 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H13" t="n">
         <v>0.0</v>
@@ -520,7 +520,7 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H14" t="n">
         <v>0.0</v>
@@ -547,7 +547,7 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.10999999940395355</v>
+        <v>0.0</v>
       </c>
       <c r="H15" t="n">
         <v>0.0</v>

</xml_diff>

<commit_message>
simplified flow by reading from beans directly and deleting mappers
</commit_message>
<xml_diff>
--- a/src/main/resources/files/results/CHAMPIONS.xlsx
+++ b/src/main/resources/files/results/CHAMPIONS.xlsx
@@ -44,46 +44,46 @@
     <t/>
   </si>
   <si>
+    <t>Lundo’s Legends</t>
+  </si>
+  <si>
+    <t>EL Onće</t>
+  </si>
+  <si>
+    <t>Samsquanches</t>
+  </si>
+  <si>
+    <t>GOD WILLS IT</t>
+  </si>
+  <si>
+    <t>Swampnuts</t>
+  </si>
+  <si>
+    <t>Splitfinger Skadoosh</t>
+  </si>
+  <si>
+    <t>Epic7</t>
+  </si>
+  <si>
     <t>rainmaker</t>
   </si>
   <si>
-    <t>Lundo’s Legends</t>
-  </si>
-  <si>
-    <t>EL Onće</t>
-  </si>
-  <si>
-    <t>GOD WILLS IT</t>
+    <t>confusion</t>
+  </si>
+  <si>
+    <t>Mac</t>
   </si>
   <si>
     <t>MillerTime</t>
   </si>
   <si>
-    <t>Samsquanches</t>
-  </si>
-  <si>
-    <t>Swampnuts</t>
-  </si>
-  <si>
-    <t>Splitfinger Skadoosh</t>
+    <t>SmokeWalkers</t>
   </si>
   <si>
     <t>Corbin Copy</t>
   </si>
   <si>
-    <t>Epic7</t>
-  </si>
-  <si>
     <t>DJ's Quality Team</t>
-  </si>
-  <si>
-    <t>confusion</t>
-  </si>
-  <si>
-    <t>SmokeWalkers</t>
-  </si>
-  <si>
-    <t>Mac</t>
   </si>
   <si>
     <t xml:space="preserve">rank </t>
@@ -186,17 +186,17 @@
         <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>124.0</v>
+        <v>133.5</v>
       </c>
       <c r="D2" t="n">
-        <v>68.0</v>
+        <v>60.0</v>
       </c>
       <c r="E2" t="n">
-        <v>56.0</v>
+        <v>73.5</v>
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -213,17 +213,17 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>120.5</v>
+        <v>132.0</v>
       </c>
       <c r="D3" t="n">
-        <v>57.5</v>
+        <v>65.5</v>
       </c>
       <c r="E3" t="n">
-        <v>63.0</v>
+        <v>66.5</v>
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H3" t="n">
         <v>0.0</v>
@@ -240,17 +240,17 @@
         <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>110.0</v>
+        <v>105.5</v>
       </c>
       <c r="D4" t="n">
-        <v>57.0</v>
+        <v>59.0</v>
       </c>
       <c r="E4" t="n">
-        <v>53.0</v>
+        <v>46.5</v>
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H4" t="n">
         <v>0.0</v>
@@ -267,17 +267,17 @@
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>106.5</v>
+        <v>100.5</v>
       </c>
       <c r="D5" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="E5" t="n">
         <v>51.0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>55.5</v>
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H5" t="n">
         <v>0.0</v>
@@ -288,23 +288,23 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5.5</v>
+        <v>5.0</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>93.5</v>
+        <v>95.0</v>
       </c>
       <c r="D6" t="n">
-        <v>52.5</v>
+        <v>39.0</v>
       </c>
       <c r="E6" t="n">
-        <v>41.0</v>
+        <v>56.0</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H6" t="n">
         <v>0.0</v>
@@ -315,23 +315,23 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5.5</v>
+        <v>6.0</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>93.5</v>
+        <v>94.5</v>
       </c>
       <c r="D7" t="n">
-        <v>49.5</v>
+        <v>39.0</v>
       </c>
       <c r="E7" t="n">
-        <v>44.0</v>
+        <v>55.5</v>
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H7" t="n">
         <v>0.0</v>
@@ -348,17 +348,17 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>85.0</v>
+        <v>89.0</v>
       </c>
       <c r="D8" t="n">
-        <v>31.5</v>
+        <v>40.0</v>
       </c>
       <c r="E8" t="n">
-        <v>53.5</v>
+        <v>49.0</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H8" t="n">
         <v>0.0</v>
@@ -375,17 +375,17 @@
         <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>82.5</v>
+        <v>81.5</v>
       </c>
       <c r="D9" t="n">
-        <v>31.5</v>
+        <v>23.0</v>
       </c>
       <c r="E9" t="n">
-        <v>51.0</v>
+        <v>58.5</v>
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H9" t="n">
         <v>0.0</v>
@@ -396,23 +396,23 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9.5</v>
+        <v>9.0</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="n">
-        <v>81.5</v>
+        <v>78.0</v>
       </c>
       <c r="D10" t="n">
-        <v>41.0</v>
+        <v>52.0</v>
       </c>
       <c r="E10" t="n">
-        <v>40.5</v>
+        <v>26.0</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H10" t="n">
         <v>0.0</v>
@@ -423,23 +423,23 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9.5</v>
+        <v>10.0</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="n">
-        <v>81.5</v>
+        <v>76.5</v>
       </c>
       <c r="D11" t="n">
-        <v>34.0</v>
+        <v>44.0</v>
       </c>
       <c r="E11" t="n">
-        <v>47.5</v>
+        <v>32.5</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H11" t="n">
         <v>0.0</v>
@@ -456,17 +456,17 @@
         <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>77.0</v>
+        <v>72.5</v>
       </c>
       <c r="D12" t="n">
-        <v>43.5</v>
+        <v>38.0</v>
       </c>
       <c r="E12" t="n">
-        <v>33.5</v>
+        <v>34.5</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H12" t="n">
         <v>0.0</v>
@@ -483,17 +483,17 @@
         <v>21</v>
       </c>
       <c r="C13" t="n">
-        <v>70.0</v>
+        <v>71.5</v>
       </c>
       <c r="D13" t="n">
-        <v>45.5</v>
+        <v>36.0</v>
       </c>
       <c r="E13" t="n">
-        <v>24.5</v>
+        <v>35.5</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H13" t="n">
         <v>0.0</v>
@@ -510,17 +510,17 @@
         <v>22</v>
       </c>
       <c r="C14" t="n">
-        <v>69.0</v>
+        <v>67.0</v>
       </c>
       <c r="D14" t="n">
-        <v>34.5</v>
+        <v>44.5</v>
       </c>
       <c r="E14" t="n">
-        <v>34.5</v>
+        <v>22.5</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H14" t="n">
         <v>0.0</v>
@@ -537,17 +537,17 @@
         <v>23</v>
       </c>
       <c r="C15" t="n">
-        <v>65.5</v>
+        <v>63.0</v>
       </c>
       <c r="D15" t="n">
-        <v>33.0</v>
+        <v>40.5</v>
       </c>
       <c r="E15" t="n">
-        <v>32.5</v>
+        <v>22.5</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.0</v>
+        <v>0.10999999940395355</v>
       </c>
       <c r="H15" t="n">
         <v>0.0</v>
@@ -585,20 +585,20 @@
         <v>1.0</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" t="n">
-        <v>68.0</v>
+        <v>65.5</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="n">
         <v>1.0</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G18" t="n">
-        <v>63.0</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="19">
@@ -606,20 +606,20 @@
         <v>2.0</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>57.5</v>
+        <v>60.0</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="n">
         <v>2.0</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G19" t="n">
-        <v>56.0</v>
+        <v>66.5</v>
       </c>
     </row>
     <row r="20">
@@ -630,17 +630,17 @@
         <v>12</v>
       </c>
       <c r="C20" t="n">
-        <v>57.0</v>
+        <v>59.0</v>
       </c>
       <c r="D20"/>
       <c r="E20" t="n">
         <v>3.0</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G20" t="n">
-        <v>55.5</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="21">
@@ -648,20 +648,20 @@
         <v>4.0</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C21" t="n">
-        <v>52.5</v>
+        <v>52.0</v>
       </c>
       <c r="D21"/>
       <c r="E21" t="n">
         <v>4.0</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G21" t="n">
-        <v>53.5</v>
+        <v>56.0</v>
       </c>
     </row>
     <row r="22">
@@ -672,17 +672,17 @@
         <v>13</v>
       </c>
       <c r="C22" t="n">
-        <v>51.0</v>
+        <v>49.5</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="n">
         <v>5.0</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G22" t="n">
-        <v>53.0</v>
+        <v>55.5</v>
       </c>
     </row>
     <row r="23">
@@ -690,17 +690,17 @@
         <v>6.0</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>49.5</v>
+        <v>44.5</v>
       </c>
       <c r="D23"/>
       <c r="E23" t="n">
         <v>6.0</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G23" t="n">
         <v>51.0</v>
@@ -711,20 +711,20 @@
         <v>7.0</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C24" t="n">
-        <v>45.5</v>
+        <v>44.0</v>
       </c>
       <c r="D24"/>
       <c r="E24" t="n">
         <v>7.0</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G24" t="n">
-        <v>47.5</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="25">
@@ -732,20 +732,20 @@
         <v>8.0</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C25" t="n">
-        <v>43.5</v>
+        <v>40.5</v>
       </c>
       <c r="D25"/>
       <c r="E25" t="n">
         <v>8.0</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G25" t="n">
-        <v>44.0</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="26">
@@ -753,62 +753,62 @@
         <v>9.0</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C26" t="n">
-        <v>41.0</v>
+        <v>40.0</v>
       </c>
       <c r="D26"/>
       <c r="E26" t="n">
         <v>9.0</v>
       </c>
       <c r="F26" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G26" t="n">
-        <v>41.0</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>10.0</v>
+        <v>10.5</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C27" t="n">
-        <v>34.5</v>
+        <v>39.0</v>
       </c>
       <c r="D27"/>
       <c r="E27" t="n">
         <v>10.0</v>
       </c>
       <c r="F27" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G27" t="n">
-        <v>40.5</v>
+        <v>34.5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>11.0</v>
+        <v>10.5</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C28" t="n">
-        <v>34.0</v>
+        <v>39.0</v>
       </c>
       <c r="D28"/>
       <c r="E28" t="n">
         <v>11.0</v>
       </c>
       <c r="F28" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G28" t="n">
-        <v>34.5</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="29">
@@ -816,62 +816,62 @@
         <v>12.0</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C29" t="n">
-        <v>33.0</v>
+        <v>38.0</v>
       </c>
       <c r="D29"/>
       <c r="E29" t="n">
         <v>12.0</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G29" t="n">
-        <v>33.5</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>13.5</v>
+        <v>13.0</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C30" t="n">
-        <v>31.5</v>
+        <v>36.0</v>
       </c>
       <c r="D30"/>
       <c r="E30" t="n">
-        <v>13.0</v>
+        <v>13.5</v>
       </c>
       <c r="F30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G30" t="n">
-        <v>32.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>13.5</v>
+        <v>14.0</v>
       </c>
       <c r="B31" t="s">
         <v>17</v>
       </c>
       <c r="C31" t="n">
-        <v>31.5</v>
+        <v>23.0</v>
       </c>
       <c r="D31"/>
       <c r="E31" t="n">
-        <v>14.0</v>
+        <v>13.5</v>
       </c>
       <c r="F31" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G31" t="n">
-        <v>24.5</v>
+        <v>22.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>